<commit_message>
Update Attendance Roster_Splunk Certified Architect_October 06-10_VC00529848.xlsx
</commit_message>
<xml_diff>
--- a/Attendance Roster_Splunk Certified Architect_October 06-10_VC00529848.xlsx
+++ b/Attendance Roster_Splunk Certified Architect_October 06-10_VC00529848.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\VK_GIT\SPLK_ARCHITECT_06_10_2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE26EA7B-059D-4912-934D-37E361203865}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B7A0AC2-893A-4B78-A905-37E381FD17BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="75">
   <si>
     <t>Start Date</t>
   </si>
@@ -170,6 +170,87 @@
   </si>
   <si>
     <t>https://cloud4.rpsconsulting.in/console/#</t>
+  </si>
+  <si>
+    <t>174.129.73.140</t>
+  </si>
+  <si>
+    <t>52.91.55.48</t>
+  </si>
+  <si>
+    <t>34.229.155.235</t>
+  </si>
+  <si>
+    <t>98.80.9.40</t>
+  </si>
+  <si>
+    <t>34.202.230.107</t>
+  </si>
+  <si>
+    <t>52.55.213.186</t>
+  </si>
+  <si>
+    <t>54.242.108.128</t>
+  </si>
+  <si>
+    <t>34.236.146.139</t>
+  </si>
+  <si>
+    <t>34.229.57.121</t>
+  </si>
+  <si>
+    <t>98.84.127.232</t>
+  </si>
+  <si>
+    <t>54.221.6.74</t>
+  </si>
+  <si>
+    <t>34.228.155.29</t>
+  </si>
+  <si>
+    <t>3.208.12.191</t>
+  </si>
+  <si>
+    <t>13.220.50.93</t>
+  </si>
+  <si>
+    <t>100.26.111.168</t>
+  </si>
+  <si>
+    <t>18.208.220.175</t>
+  </si>
+  <si>
+    <t>34.224.93.22</t>
+  </si>
+  <si>
+    <t>54.227.96.203</t>
+  </si>
+  <si>
+    <t>23.20.122.36</t>
+  </si>
+  <si>
+    <t>3.91.66.211</t>
+  </si>
+  <si>
+    <t>3.94.115.94</t>
+  </si>
+  <si>
+    <t>34.234.63.205</t>
+  </si>
+  <si>
+    <t>54.90.72.181</t>
+  </si>
+  <si>
+    <t xml:space="preserve">54.167.22.31  </t>
+  </si>
+  <si>
+    <t>IP1</t>
+  </si>
+  <si>
+    <t>IP2</t>
+  </si>
+  <si>
+    <t>ubuntu</t>
   </si>
 </sst>
 </file>
@@ -617,12 +698,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -632,6 +707,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -928,10 +1009,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="30"/>
+      <c r="C1" s="35"/>
       <c r="D1" s="20"/>
       <c r="E1" s="20"/>
       <c r="F1" s="20"/>
@@ -1213,10 +1294,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FFDF7D1-DA1C-4502-A043-BA17F7696C93}">
-  <dimension ref="B8:E23"/>
+  <dimension ref="B8:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="J9" sqref="J9:K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1224,167 +1305,300 @@
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="38.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B8" s="35" t="s">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B8" s="33" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B11" s="31" t="s">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B11" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="32"/>
-      <c r="D11" s="32" t="s">
+      <c r="C11" s="30"/>
+      <c r="D11" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="E11" s="32" t="s">
+      <c r="E11" s="30" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B12" s="33" t="s">
+      <c r="F11" s="32"/>
+      <c r="G11" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="H11" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="I11" s="30" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B12" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="34"/>
-      <c r="D12" s="34" t="s">
+      <c r="C12" s="32"/>
+      <c r="D12" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="E12" s="34" t="s">
+      <c r="E12" s="32" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F12" s="32"/>
+      <c r="G12" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="H12" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="I12" s="32" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B13" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="34"/>
-      <c r="D13" s="34" t="s">
+      <c r="C13" s="32"/>
+      <c r="D13" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="32" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F13" s="32"/>
+      <c r="G13" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="H13" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="I13" s="32" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B14" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="34"/>
-      <c r="D14" s="34" t="s">
+      <c r="C14" s="32"/>
+      <c r="D14" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="32" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F14" s="32"/>
+      <c r="G14" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="H14" s="32" t="s">
+        <v>61</v>
+      </c>
+      <c r="I14" s="32" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B15" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="34"/>
-      <c r="D15" s="34" t="s">
+      <c r="C15" s="32"/>
+      <c r="D15" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="32" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F15" s="32"/>
+      <c r="G15" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="H15" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="I15" s="32" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B16" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="34"/>
-      <c r="D16" s="34" t="s">
+      <c r="C16" s="32"/>
+      <c r="D16" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="32" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F16" s="32"/>
+      <c r="G16" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="H16" s="32" t="s">
+        <v>63</v>
+      </c>
+      <c r="I16" s="32" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B17" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="34"/>
-      <c r="D17" s="34" t="s">
+      <c r="C17" s="32"/>
+      <c r="D17" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="32" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F17" s="32"/>
+      <c r="G17" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="H17" s="32" t="s">
+        <v>64</v>
+      </c>
+      <c r="I17" s="32" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B18" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="34"/>
-      <c r="D18" s="34" t="s">
+      <c r="C18" s="32"/>
+      <c r="D18" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="32" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F18" s="32"/>
+      <c r="G18" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="H18" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="I18" s="32" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B19" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="34"/>
-      <c r="D19" s="34" t="s">
+      <c r="C19" s="32"/>
+      <c r="D19" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="32" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F19" s="32"/>
+      <c r="G19" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="H19" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="I19" s="32" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B20" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="34"/>
-      <c r="D20" s="34" t="s">
+      <c r="C20" s="32"/>
+      <c r="D20" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="32" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F20" s="32"/>
+      <c r="G20" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="H20" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="I20" s="32" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B21" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="34"/>
-      <c r="D21" s="34" t="s">
+      <c r="C21" s="32"/>
+      <c r="D21" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="32" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F21" s="32"/>
+      <c r="G21" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="H21" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="I21" s="32" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B22" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="C22" s="34"/>
-      <c r="D22" s="34" t="s">
+      <c r="C22" s="32"/>
+      <c r="D22" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="32" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F22" s="32"/>
+      <c r="G22" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="H22" s="32" t="s">
+        <v>69</v>
+      </c>
+      <c r="I22" s="32" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B23" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="C23" s="34"/>
-      <c r="D23" s="34" t="s">
+      <c r="C23" s="32"/>
+      <c r="D23" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="E23" s="34" t="s">
+      <c r="E23" s="32" t="s">
         <v>34</v>
+      </c>
+      <c r="F23" s="32"/>
+      <c r="G23" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="H23" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="I23" s="32" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>